<commit_message>
Send email with data from excel
</commit_message>
<xml_diff>
--- a/cellfone & acessories.xlsx
+++ b/cellfone & acessories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev\Documents\UiPath\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4E7DD6-A084-47BE-8803-F76D50150DCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187251E9-80D6-47D6-AC2B-F64B70817529}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2640" yWindow="2640" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -488,9 +488,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="134.85546875" customWidth="1"/>
+    <col min="2" max="2" width="144.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>